<commit_message>
Add visualization with highcharts in the line files
</commit_message>
<xml_diff>
--- a/user_files/hilarytn/facility1/source1/line_8.xlsx
+++ b/user_files/hilarytn/facility1/source1/line_8.xlsx
@@ -58,12 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,10 +507,10 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
+          <t>44bb2153-845f-4543-8e0b-e127667e7e30</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -540,10 +541,10 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
+          <t>44bb2153-845f-4543-8e0b-e127667e7e30</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -574,10 +575,10 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
+          <t>44bb2153-845f-4543-8e0b-e127667e7e30</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -608,10 +609,10 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
+          <t>44bb2153-845f-4543-8e0b-e127667e7e30</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -642,10 +643,10 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
+          <t>44bb2153-845f-4543-8e0b-e127667e7e30</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -676,214 +677,10 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Line:8 Stage:1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>01/09/2024</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pri cl LA</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>45300.42056299769</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>45300.42067873842</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Line:8 Stage:1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>01/09/2024</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>pri pH HA</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>45300.65476473379</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>45300.65488047454</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Line:8 Stage:1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>01/09/2024</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>pri cl LA</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>45300.42056299769</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>45300.42067873842</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Line:8 Stage:1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>01/09/2024</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>pri pH HA</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>45300.65476473379</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>45300.65488047454</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Line:8 Stage:1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>01/09/2024</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>pri cl LA</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>45300.42056299769</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>45300.42067873842</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Line:8 Stage:1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>01/09/2024</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>pri pH HA</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>45300.65476473379</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>45300.65488047454</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>ba38b901-e613-4dbc-8708-5a8cc1c7f21e</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
+          <t>44bb2153-845f-4543-8e0b-e127667e7e30</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add line data to all facility line responses
</commit_message>
<xml_diff>
--- a/user_files/hilarytn/facility1/source1/line_8.xlsx
+++ b/user_files/hilarytn/facility1/source1/line_8.xlsx
@@ -58,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -510,7 +509,7 @@
           <t>c4f1636a-d92c-45e5-82c9-d146dc727e93</t>
         </is>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -544,7 +543,7 @@
           <t>c4f1636a-d92c-45e5-82c9-d146dc727e93</t>
         </is>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>